<commit_message>
Options Bar replaced by Menu
</commit_message>
<xml_diff>
--- a/Appetite - Test Cases - Sprint 3.xlsx
+++ b/Appetite - Test Cases - Sprint 3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandoito/Documents/GitHub/722/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandoito/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="2360" windowWidth="25600" windowHeight="14520" tabRatio="821"/>
+    <workbookView xWindow="1920" yWindow="1940" windowWidth="25600" windowHeight="14520" tabRatio="821"/>
   </bookViews>
   <sheets>
     <sheet name="Patient-Clinical Data" sheetId="122" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>TC1</t>
   </si>
@@ -172,18 +172,6 @@
 Search result will include restaurants within this range from the current position of the user.</t>
   </si>
   <si>
-    <t xml:space="preserve">Restaurants nearby:
-There will be an Options Bar at the top of the screen. </t>
-  </si>
-  <si>
-    <t>Restaurants nearby:
-This bar will include several options that can be browse by scrolling horizontally.</t>
-  </si>
-  <si>
-    <t>Restaurants nearby:
-When user presses "Range" button, a Popup Screen will appear showing a slider bar to setup a value for range.</t>
-  </si>
-  <si>
     <t>Restaurants nearby:
 This value will be saved in User Preferences.</t>
   </si>
@@ -197,33 +185,6 @@
   <si>
     <t xml:space="preserve">"Search range (km)" window appears with the slide button in the middle. Range starts from 0 km to 100 km. CANCEL and OK options appear.
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose Range from main menu;
-Slide the bar with the desired distance range (in kilometer);
-Hit OK </t>
-  </si>
-  <si>
-    <t>Under development</t>
-  </si>
-  <si>
-    <t>Choose List from main menu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose List from main menu;
-</t>
-  </si>
-  <si>
-    <t>Option Bar might have the following options:
-- Option 1;
-- Option 2;
-- Option 3.</t>
-  </si>
-  <si>
-    <t>The Options Bar might appear on the top of the screen.</t>
-  </si>
-  <si>
-    <t>Map is updated with the restaurants nearby within the selected distance range.</t>
   </si>
   <si>
     <t xml:space="preserve">Choose Range from main menu;
@@ -232,6 +193,43 @@
   </si>
   <si>
     <t>The last distance might apper (30 km).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose the Menu on the top right of the main screen;
+</t>
+  </si>
+  <si>
+    <t>The menu might have the following options:
+Range
+Map
+List</t>
+  </si>
+  <si>
+    <t>Restaurants nearby:
+There will have a Menu at the top right of the screen.</t>
+  </si>
+  <si>
+    <t>Open the application</t>
+  </si>
+  <si>
+    <t>The menu will be represented with three vertical bullets on the top-right in the screen.</t>
+  </si>
+  <si>
+    <t>Choose Range from main menu;
+Slide the bar with the desired distance range (in kilometer);
+Hit OK;
+Choose List from the menu.</t>
+  </si>
+  <si>
+    <t>Restaurants nearby:
+By pressing "Range" button, a Popup Screen will appear showing a slider bar to setup a value for range.</t>
+  </si>
+  <si>
+    <t>Restaurants nearby:
+The Menu will include the options Range, Map and List.</t>
+  </si>
+  <si>
+    <t>The distance might be within the range specified in the "Range" settings.</t>
   </si>
 </sst>
 </file>
@@ -959,15 +957,36 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -978,27 +997,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3608,7 +3606,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3631,17 +3629,17 @@
       <c r="A2" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="58"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
       <c r="E2" s="39"/>
       <c r="F2" s="39"/>
       <c r="G2" s="39"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
       <c r="K2" s="40"/>
       <c r="L2" s="40"/>
     </row>
@@ -3660,9 +3658,9 @@
       <c r="E3" s="44"/>
       <c r="F3" s="44"/>
       <c r="G3" s="44"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
       <c r="K3" s="40"/>
       <c r="L3" s="40"/>
     </row>
@@ -3671,30 +3669,30 @@
         <v>7</v>
       </c>
       <c r="B4" s="46">
-        <f>COUNTIF(I8:I11,"Fail")</f>
+        <f>COUNTIF(I11:I12,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C4" s="47" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="48">
-        <f>COUNTA(A8:A24)</f>
-        <v>11</v>
+        <f>COUNTA(A11:A24)</f>
+        <v>8</v>
       </c>
       <c r="E4" s="49"/>
       <c r="F4" s="49"/>
       <c r="G4" s="49"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
       <c r="K4" s="40"/>
       <c r="L4" s="40"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="61"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
+      <c r="A5" s="68"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
       <c r="E5" s="44"/>
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
@@ -3705,46 +3703,46 @@
       <c r="L5" s="40"/>
     </row>
     <row r="6" spans="1:12" s="33" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="66"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="62" t="s">
+      <c r="E6" s="60"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="H6" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="59" t="s">
+      <c r="I6" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="59" t="s">
+      <c r="J6" s="58" t="s">
         <v>25</v>
       </c>
       <c r="K6" s="40"/>
       <c r="L6" s="40"/>
     </row>
     <row r="7" spans="1:12" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="59"/>
-      <c r="B7" s="64"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="50"/>
       <c r="L7" s="50"/>
     </row>
@@ -3753,18 +3751,18 @@
         <v>0</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D8" s="54" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E8" s="55"/>
       <c r="F8" s="56"/>
       <c r="G8" s="51" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H8" s="52">
         <v>43170</v>
@@ -3776,107 +3774,107 @@
       <c r="K8" s="53"/>
       <c r="L8" s="53"/>
     </row>
-    <row r="9" spans="1:12" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" s="2" customFormat="1" ht="85.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="51" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C9" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="54" t="s">
         <v>45</v>
-      </c>
-      <c r="D9" s="54" t="s">
-        <v>51</v>
       </c>
       <c r="E9" s="55"/>
       <c r="F9" s="56"/>
       <c r="G9" s="51" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H9" s="52">
         <v>43170</v>
       </c>
       <c r="I9" s="51" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="J9" s="51"/>
       <c r="K9" s="53"/>
       <c r="L9" s="53"/>
     </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="51" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E10" s="55"/>
       <c r="F10" s="56"/>
       <c r="G10" s="51" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H10" s="52">
         <v>43170</v>
       </c>
       <c r="I10" s="51" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="J10" s="51"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
     </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" ht="85.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" s="2" customFormat="1" ht="54" x14ac:dyDescent="0.15">
       <c r="A11" s="51" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="51" t="s">
-        <v>48</v>
-      </c>
       <c r="D11" s="54" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E11" s="55"/>
       <c r="F11" s="56"/>
       <c r="G11" s="51" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H11" s="52">
         <v>43170</v>
       </c>
       <c r="I11" s="51" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="J11" s="51"/>
       <c r="K11" s="53"/>
       <c r="L11" s="53"/>
     </row>
-    <row r="12" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.15">
       <c r="A12" s="51" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D12" s="54" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E12" s="55"/>
       <c r="F12" s="56"/>
       <c r="G12" s="51" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H12" s="52">
         <v>43170</v>
@@ -3885,26 +3883,26 @@
         <v>26</v>
       </c>
       <c r="J12" s="51"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
     </row>
     <row r="13" spans="1:12" ht="72" x14ac:dyDescent="0.15">
       <c r="A13" s="51" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D13" s="54" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E13" s="55"/>
       <c r="F13" s="56"/>
       <c r="G13" s="51" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H13" s="52">
         <v>43165</v>
@@ -4082,13 +4080,13 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D6:F7"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J6:J7"/>
@@ -4099,19 +4097,19 @@
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D10:F10"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D8:F8"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D6:F7"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4235,7 +4233,7 @@
       </c>
       <c r="G8" s="31">
         <f>'Patient-Clinical Data'!D4</f>
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
@@ -4267,7 +4265,7 @@
       </c>
       <c r="G10" s="25">
         <f>SUM(G6:G9)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
TC7 Added in the Test Case - Sprint 3 spreadsheet
</commit_message>
<xml_diff>
--- a/Appetite - Test Cases - Sprint 3.xlsx
+++ b/Appetite - Test Cases - Sprint 3.xlsx
@@ -5,18 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandoito/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandoito/Documents/GitHub/722/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1940" windowWidth="25600" windowHeight="14520" tabRatio="821"/>
   </bookViews>
   <sheets>
-    <sheet name="Patient-Clinical Data" sheetId="122" r:id="rId1"/>
-    <sheet name="Test Report" sheetId="107" r:id="rId2"/>
+    <sheet name="Sprint 3" sheetId="122" r:id="rId1"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
     <definedName name="Access">[1]Validation!$E$2:$E$223</definedName>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>TC1</t>
   </si>
@@ -67,46 +66,15 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>Date</t>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
     <t>Test Case Description</t>
   </si>
   <si>
     <t>Result</t>
   </si>
   <si>
-    <t>Note:</t>
-  </si>
-  <si>
-    <t>TEST REPORT</t>
-  </si>
-  <si>
     <t>Test Case Procedure</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Module code</t>
-  </si>
-  <si>
-    <t>Number of  test cases</t>
-  </si>
-  <si>
-    <t>Sub total</t>
-  </si>
-  <si>
-    <t>Test coverage</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>Test successful coverage</t>
-  </si>
-  <si>
     <t>Test date</t>
   </si>
   <si>
@@ -141,9 +109,6 @@
   </si>
   <si>
     <t>Tested By</t>
-  </si>
-  <si>
-    <t>Patient-Clinical Data</t>
   </si>
   <si>
     <r>
@@ -231,15 +196,22 @@
   <si>
     <t>The distance might be within the range specified in the "Range" settings.</t>
   </si>
+  <si>
+    <t>Restaurants nearby:
+Show nearby restaurants close to the current user location (i.e. Centennial College)</t>
+  </si>
+  <si>
+    <t>Open the application and click / tap onto a restaurant nearby the user location (i.e. Centennial College) in the map.</t>
+  </si>
+  <si>
+    <t>The Restaurant details (i.e. restaurant name appears)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-  </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -279,50 +251,6 @@
       <color indexed="8"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="8"/>
@@ -374,7 +302,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,18 +317,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="18"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="56"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -484,141 +406,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -813,198 +600,123 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Functional Test Case v1.0" xfId="1"/>
-    <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="2"/>
-    <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="3"/>
+    <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="1"/>
+    <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3606,487 +3318,499 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" style="34" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="42.1640625" customWidth="1"/>
     <col min="4" max="4" width="23.83203125" customWidth="1"/>
     <col min="6" max="6" width="27.83203125" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="7"/>
-    <col min="10" max="10" width="18" style="36" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="3"/>
+    <col min="10" max="10" width="18" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="37"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="65" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
+      <c r="A2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="43">
+      <c r="A3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="14">
         <f>COUNTIF(I7:I682,"Pending")</f>
         <v>0</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="17">
         <f>COUNTIF(I11:I12,"Fail")</f>
         <v>0</v>
       </c>
-      <c r="C4" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="48">
+      <c r="C4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="19">
         <f>COUNTA(A11:A24)</f>
         <v>8</v>
       </c>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="68"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:12" s="33" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="57" t="s">
+    <row r="6" spans="1:12" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="58" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="69" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="58" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
+      <c r="J6" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="58"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
+    <row r="7" spans="1:12" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="30"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" ht="54" x14ac:dyDescent="0.15">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="52">
-        <v>43170</v>
-      </c>
-      <c r="I8" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="51"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
+      <c r="B8" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="23">
+        <v>43172</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="22"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" ht="85.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="51" t="s">
+      <c r="B9" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="52">
-        <v>43170</v>
-      </c>
-      <c r="I9" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="51"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
+      <c r="C9" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="23">
+        <v>43172</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="22"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
     </row>
     <row r="10" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="51" t="s">
+      <c r="B10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="52">
+      <c r="C10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="23">
         <v>43170</v>
       </c>
-      <c r="I10" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="51"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
+      <c r="I10" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="22"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:12" s="2" customFormat="1" ht="54" x14ac:dyDescent="0.15">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="55"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="52">
+      <c r="B11" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="23">
         <v>43170</v>
       </c>
-      <c r="I11" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="51"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
+      <c r="I11" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="22"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.15">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="55"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="52">
-        <v>43170</v>
-      </c>
-      <c r="I12" s="51" t="s">
+      <c r="B12" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="51"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
+      <c r="C12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="23">
+        <v>43172</v>
+      </c>
+      <c r="I12" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="22"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
     </row>
     <row r="13" spans="1:12" ht="72" x14ac:dyDescent="0.15">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="51" t="s">
+      <c r="B13" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="23">
+        <v>43170</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="22"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" ht="72" x14ac:dyDescent="0.15">
+      <c r="A14" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="C14" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="52">
-        <v>43165</v>
-      </c>
-      <c r="I13" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="51"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-    </row>
-    <row r="14" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A14" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
+      <c r="D14" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="23">
+        <v>43172</v>
+      </c>
+      <c r="I14" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="22"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A15" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
+      <c r="A15" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A16" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
+      <c r="A16" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A17" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
+      <c r="A17" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
     </row>
     <row r="18" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A18" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
+      <c r="A18" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
     </row>
     <row r="19" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A19" s="51"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
     </row>
     <row r="20" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A20" s="51"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A21" s="51"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
     </row>
     <row r="22" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A22" s="51"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
     </row>
     <row r="23" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A23" s="51"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
     </row>
     <row r="24" spans="1:12" ht="18" x14ac:dyDescent="0.15">
-      <c r="A24" s="51"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D6:F7"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J6:J7"/>
@@ -4103,218 +3827,17 @@
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D6:F7"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
   </mergeCells>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="A7" s="8"/>
-      <c r="B7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29">
-        <v>1</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="31">
-        <f>'Patient-Clinical Data'!B3</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="30">
-        <f>'Patient-Clinical Data'!B4</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="30">
-        <f>'Patient-Clinical Data'!D3</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="31">
-        <f>'Patient-Clinical Data'!D4</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="7"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="17"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="7"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="24">
-        <f>SUM(D6:D9)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="24">
-        <f>SUM(E6:E9)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="24">
-        <f>SUM(F6:F9)</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="25">
-        <f>SUM(G6:G9)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="7"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="12">
-        <f>(D10+E10)*100/G10</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="12">
-        <f>D10*100/G10</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="13"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="9"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;L&amp;"Tahoma,Regular"&amp;8 02ae-BM/PM/HDCV/FSOFT v1/0</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Test case is added for rating
</commit_message>
<xml_diff>
--- a/Appetite - Test Cases - Sprint 3.xlsx
+++ b/Appetite - Test Cases - Sprint 3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandoito/Documents/GitHub/722/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fatihinan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EC89A7-273C-B644-9867-6D02BEDFEFFC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1940" windowWidth="25600" windowHeight="14520" tabRatio="821"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32640" windowHeight="20540" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 3" sheetId="122" r:id="rId1"/>
@@ -27,7 +28,7 @@
     <definedName name="Port">[1]Validation!$F$2:$F$40</definedName>
     <definedName name="VancoProducts">[1]Validation!$B$2:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>TC1</t>
   </si>
@@ -206,21 +207,28 @@
   <si>
     <t>The Restaurant details (i.e. restaurant name appears)</t>
   </si>
+  <si>
+    <t>Check rating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose two restaurants on the application and check their rating on Yelp.com
+</t>
+  </si>
+  <si>
+    <t>The ratings match</t>
+  </si>
+  <si>
+    <t>Fatih</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
       <charset val="128"/>
     </font>
     <font>
@@ -603,120 +611,120 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="1"/>
-    <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="2"/>
+    <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3311,17 +3319,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" style="6" customWidth="1"/>
@@ -3334,28 +3342,28 @@
     <col min="10" max="10" width="18" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="18" thickBot="1">
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="36">
       <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="18">
       <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
@@ -3370,13 +3378,13 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="19" thickBot="1">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
@@ -3394,17 +3402,17 @@
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="18">
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -3414,51 +3422,51 @@
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:12" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:12" s="5" customFormat="1" ht="18">
+      <c r="A6" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="33" t="s">
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="29" t="s">
         <v>15</v>
       </c>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
+    <row r="7" spans="1:12" s="4" customFormat="1" ht="18">
+      <c r="A7" s="29"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
     </row>
-    <row r="8" spans="1:12" s="2" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="54">
       <c r="A8" s="22" t="s">
         <v>0</v>
       </c>
@@ -3486,7 +3494,7 @@
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
     </row>
-    <row r="9" spans="1:12" s="2" customFormat="1" ht="85.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" s="2" customFormat="1" ht="85.75" customHeight="1">
       <c r="A9" s="22" t="s">
         <v>1</v>
       </c>
@@ -3514,7 +3522,7 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
     </row>
-    <row r="10" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="72" customHeight="1">
       <c r="A10" s="22" t="s">
         <v>2</v>
       </c>
@@ -3542,7 +3550,7 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" s="2" customFormat="1" ht="54">
       <c r="A11" s="22" t="s">
         <v>3</v>
       </c>
@@ -3570,7 +3578,7 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
     </row>
-    <row r="12" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" s="2" customFormat="1" ht="90">
       <c r="A12" s="22" t="s">
         <v>4</v>
       </c>
@@ -3598,7 +3606,7 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
     </row>
-    <row r="13" spans="1:12" ht="72" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="72">
       <c r="A13" s="22" t="s">
         <v>5</v>
       </c>
@@ -3626,7 +3634,7 @@
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="1:12" ht="72" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="72">
       <c r="A14" s="22" t="s">
         <v>6</v>
       </c>
@@ -3654,23 +3662,35 @@
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
     </row>
-    <row r="15" spans="1:12" ht="18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="72">
       <c r="A15" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="25"/>
+      <c r="B15" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>47</v>
+      </c>
       <c r="E15" s="26"/>
       <c r="F15" s="27"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="22"/>
+      <c r="G15" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="23">
+        <v>43172</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>16</v>
+      </c>
       <c r="J15" s="22"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" ht="18">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
@@ -3686,7 +3706,7 @@
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="1:12" ht="18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" ht="18">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
@@ -3702,7 +3722,7 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="1:12" ht="18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" ht="18">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
@@ -3718,7 +3738,7 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="1:12" ht="18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" ht="18">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -3732,7 +3752,7 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="1:12" ht="18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" ht="18">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -3746,7 +3766,7 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="21" spans="1:12" ht="18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" ht="18">
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
@@ -3760,7 +3780,7 @@
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
     </row>
-    <row r="22" spans="1:12" ht="18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" ht="18">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
@@ -3774,7 +3794,7 @@
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
     </row>
-    <row r="23" spans="1:12" ht="18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" ht="18">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
@@ -3788,7 +3808,7 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="1:12" ht="18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" ht="18">
       <c r="A24" s="22"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
@@ -3804,13 +3824,13 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D6:F7"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J6:J7"/>
@@ -3827,15 +3847,15 @@
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D6:F7"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>